<commit_message>
Fixes #10 : Show all bought items, show correct vat
</commit_message>
<xml_diff>
--- a/Documents/Efam Tasks and Hours 2016.xlsx
+++ b/Documents/Efam Tasks and Hours 2016.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="299"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="299" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="August 2016" sheetId="4" r:id="rId1"/>
+    <sheet name="September 2016" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -76,6 +77,12 @@
   </si>
   <si>
     <t>Issue #10 &amp; #19</t>
+  </si>
+  <si>
+    <t>Issue 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show all bought items, show correct vat </t>
   </si>
 </sst>
 </file>
@@ -459,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -674,4 +681,153 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="E3" s="3">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3">
+        <f>SUM(D3:D39)</f>
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
+        <f>E3-F3</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="30">
+      <c r="A6" s="4">
+        <v>42614</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="4"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="4"/>
+      <c r="C21" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
This closes #11, closes #15
</commit_message>
<xml_diff>
--- a/Documents/Efam Tasks and Hours 2016.xlsx
+++ b/Documents/Efam Tasks and Hours 2016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -83,6 +83,21 @@
   </si>
   <si>
     <t xml:space="preserve">Show all bought items, show correct vat </t>
+  </si>
+  <si>
+    <t>Analytics</t>
+  </si>
+  <si>
+    <t>Intergrate analytics</t>
+  </si>
+  <si>
+    <t>3G transition to live account</t>
+  </si>
+  <si>
+    <t>Issue 15 / 11</t>
+  </si>
+  <si>
+    <t>Manage products on website / new orders not being showed</t>
   </si>
 </sst>
 </file>
@@ -466,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -685,10 +700,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,12 +750,12 @@
         <v>36</v>
       </c>
       <c r="F3" s="3">
-        <f>SUM(D3:D39)</f>
-        <v>3</v>
+        <f>SUM(D3:D43)</f>
+        <v>16</v>
       </c>
       <c r="G3" s="3">
         <f>E3-F3</f>
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -772,40 +787,83 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="5"/>
+    <row r="8" spans="1:9" ht="30">
+      <c r="A8" s="4">
+        <v>42615</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="4">
+        <v>42620</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="30">
+      <c r="A12" s="4">
+        <v>42621</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="4"/>
+    <row r="14" spans="1:9" ht="45">
+      <c r="A14" s="4">
+        <v>42626</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4"/>
@@ -813,19 +871,34 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4"/>
-      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4"/>
-      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4"/>
       <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4"/>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4"/>
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4"/>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4"/>
+      <c r="C25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
This closes #7, closes #8, closes #58
</commit_message>
<xml_diff>
--- a/Documents/Efam Tasks and Hours 2016.xlsx
+++ b/Documents/Efam Tasks and Hours 2016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Manage products on website / new orders not being showed</t>
+  </si>
+  <si>
+    <t>Issue 7/8/58</t>
+  </si>
+  <si>
+    <t>Redirect app to show icons and images on e-fam server</t>
   </si>
 </sst>
 </file>
@@ -703,7 +709,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -751,11 +757,11 @@
       </c>
       <c r="F3" s="3">
         <f>SUM(D3:D43)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G3" s="3">
         <f>E3-F3</f>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -858,9 +864,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
+    <row r="15" spans="1:9" ht="45">
+      <c r="A15" s="4">
+        <v>42627</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4"/>

</xml_diff>

<commit_message>
Dry Baking goods image showing. Supermarket Right- Here removed. Fix Company token. Cash on delivery doesn't reflect on 3G
</commit_message>
<xml_diff>
--- a/Documents/Efam Tasks and Hours 2016.xlsx
+++ b/Documents/Efam Tasks and Hours 2016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -100,10 +100,19 @@
     <t>Manage products on website / new orders not being showed</t>
   </si>
   <si>
-    <t>Issue 7/8/58</t>
-  </si>
-  <si>
     <t>Redirect app to show icons and images on e-fam server</t>
+  </si>
+  <si>
+    <t>Go through the app in meeting, make impropt changes as discussed in the meeting</t>
+  </si>
+  <si>
+    <t>Issue 7/8</t>
+  </si>
+  <si>
+    <t>Issue 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dry Baking goods image showing. Supermarket Right- Here removed. Fix Company token. Cash on delivery doesn't reflect on 3G</t>
   </si>
 </sst>
 </file>
@@ -487,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -706,10 +715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -756,12 +765,12 @@
         <v>36</v>
       </c>
       <c r="F3" s="3">
-        <f>SUM(D3:D43)</f>
-        <v>18</v>
+        <f>SUM(D3:D47)</f>
+        <v>27</v>
       </c>
       <c r="G3" s="3">
         <f>E3-F3</f>
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -864,57 +873,105 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45">
-      <c r="A15" s="4">
+    <row r="15" spans="1:9">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="45">
+      <c r="A16" s="4">
         <v>42627</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" ht="60">
+      <c r="A18" s="4">
+        <v>42629</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D15">
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" ht="60">
+      <c r="A20" s="4">
+        <v>42634</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="4"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3">
+    <row r="22" spans="1:4" ht="90">
+      <c r="A22" s="4">
+        <v>42634</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="4"/>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3">
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" s="4"/>
       <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="4"/>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="4"/>
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="4"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="4"/>
+      <c r="C29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>